<commit_message>
Comentarios para trabajar en cambios de nombres
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_ThermalGEN_CurrentOilfield.xlsx
+++ b/SubRES_TMPL/SubRES_ThermalGEN_CurrentOilfield.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JULIAN\Pictures\TIMES-O-G-B\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CARMEN\Pictures\ModeloTIMESOG\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDD2D66-B2EE-472D-AFB8-778CC112FC1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96414323-301A-4DD5-96C7-AB8B73D96DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COMM&amp;PROCESS" sheetId="1" r:id="rId1"/>
@@ -30,8 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1105,11 +1103,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="\Te\x\t"/>
-    <numFmt numFmtId="165" formatCode="0.0%"/>
-    <numFmt numFmtId="166" formatCode="0.000000"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="\Te\x\t"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="0.000000"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1432,28 +1430,28 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1475,7 +1473,7 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1500,7 +1498,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1514,9 +1512,6 @@
     </xf>
     <xf numFmtId="2" fontId="5" fillId="3" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="15" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1540,9 +1535,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="6" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1832,30 +1830,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D3:AA106"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="E7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Y50" sqref="Y50"/>
+    <sheetView showGridLines="0" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="30.33203125" customWidth="1"/>
-    <col min="7" max="7" width="58.88671875" customWidth="1"/>
-    <col min="17" max="17" width="36.5546875" customWidth="1"/>
-    <col min="18" max="18" width="15.5546875" customWidth="1"/>
-    <col min="19" max="19" width="16.5546875" customWidth="1"/>
-    <col min="20" max="20" width="24.6640625" customWidth="1"/>
-    <col min="21" max="21" width="11.6640625" customWidth="1"/>
-    <col min="22" max="22" width="13.88671875" customWidth="1"/>
-    <col min="23" max="23" width="12.33203125" customWidth="1"/>
-    <col min="24" max="26" width="15.77734375" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" customWidth="1"/>
+    <col min="7" max="7" width="58.85546875" customWidth="1"/>
+    <col min="17" max="17" width="36.5703125" customWidth="1"/>
+    <col min="18" max="18" width="15.5703125" customWidth="1"/>
+    <col min="19" max="19" width="16.5703125" customWidth="1"/>
+    <col min="20" max="20" width="24.7109375" customWidth="1"/>
+    <col min="21" max="21" width="11.7109375" customWidth="1"/>
+    <col min="22" max="22" width="13.85546875" customWidth="1"/>
+    <col min="23" max="23" width="12.28515625" customWidth="1"/>
+    <col min="24" max="26" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D3" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1884,7 +1882,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="4:12" ht="42.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="4:12" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
@@ -1913,7 +1911,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="4:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D6" s="3" t="s">
         <v>18</v>
       </c>
@@ -1926,7 +1924,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D7" s="24" t="s">
         <v>88</v>
       </c>
@@ -1947,7 +1945,7 @@
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D8" s="24"/>
       <c r="E8" s="24"/>
       <c r="F8" s="25" t="s">
@@ -1966,7 +1964,7 @@
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
       <c r="F9" s="25" t="s">
@@ -1985,7 +1983,7 @@
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
       <c r="F10" s="25" t="s">
@@ -2004,7 +2002,7 @@
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
       <c r="F11" s="25" t="s">
@@ -2023,7 +2021,7 @@
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D12" s="24"/>
       <c r="E12" s="24"/>
       <c r="F12" s="25" t="s">
@@ -2042,7 +2040,7 @@
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D13" s="24"/>
       <c r="E13" s="24"/>
       <c r="F13" s="25" t="s">
@@ -2061,7 +2059,7 @@
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D14" s="24"/>
       <c r="E14" s="24"/>
       <c r="F14" s="25" t="s">
@@ -2080,7 +2078,7 @@
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D15" s="24"/>
       <c r="E15" s="24"/>
       <c r="F15" s="25" t="s">
@@ -2099,7 +2097,7 @@
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D16" s="24"/>
       <c r="E16" s="24"/>
       <c r="F16" s="25" t="s">
@@ -2118,7 +2116,7 @@
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D17" s="24"/>
       <c r="E17" s="24"/>
       <c r="F17" s="25" t="s">
@@ -2137,7 +2135,7 @@
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D18" s="24"/>
       <c r="E18" s="24"/>
       <c r="F18" s="25" t="s">
@@ -2156,7 +2154,7 @@
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D19" s="24"/>
       <c r="E19" s="24"/>
       <c r="F19" s="25" t="s">
@@ -2175,7 +2173,7 @@
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D20" s="24"/>
       <c r="E20" s="24"/>
       <c r="F20" s="25" t="s">
@@ -2194,7 +2192,7 @@
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D21" s="24"/>
       <c r="E21" s="24"/>
       <c r="F21" s="25" t="s">
@@ -2213,7 +2211,7 @@
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
     </row>
-    <row r="22" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D22" s="24"/>
       <c r="E22" s="24"/>
       <c r="F22" s="25" t="s">
@@ -2232,7 +2230,7 @@
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
     </row>
-    <row r="23" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D23" s="24"/>
       <c r="E23" s="24"/>
       <c r="F23" s="25" t="s">
@@ -2251,7 +2249,7 @@
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
     </row>
-    <row r="24" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D24" s="24"/>
       <c r="E24" s="24"/>
       <c r="F24" s="25" t="s">
@@ -2270,7 +2268,7 @@
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
     </row>
-    <row r="25" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D25" s="24"/>
       <c r="E25" s="24"/>
       <c r="F25" s="25" t="s">
@@ -2289,7 +2287,7 @@
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
     </row>
-    <row r="26" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D26" s="24"/>
       <c r="E26" s="24"/>
       <c r="F26" s="25" t="s">
@@ -2308,7 +2306,7 @@
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
     </row>
-    <row r="27" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D27" s="24"/>
       <c r="E27" s="24"/>
       <c r="F27" s="25" t="s">
@@ -2327,7 +2325,7 @@
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
     </row>
-    <row r="28" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D28" s="24"/>
       <c r="E28" s="24"/>
       <c r="F28" s="25" t="s">
@@ -2346,7 +2344,7 @@
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
     </row>
-    <row r="29" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D29" s="24"/>
       <c r="E29" s="24"/>
       <c r="F29" s="25" t="s">
@@ -2365,7 +2363,7 @@
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
     </row>
-    <row r="30" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D30" s="24"/>
       <c r="E30" s="24"/>
       <c r="F30" s="25" t="s">
@@ -2384,7 +2382,7 @@
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
     </row>
-    <row r="31" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D31" s="24"/>
       <c r="E31" s="24"/>
       <c r="F31" s="25" t="s">
@@ -2403,7 +2401,7 @@
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
     </row>
-    <row r="32" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D32" s="24"/>
       <c r="E32" s="24"/>
       <c r="F32" s="25" t="s">
@@ -2422,7 +2420,7 @@
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
     </row>
-    <row r="33" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D33" s="24"/>
       <c r="E33" s="24"/>
       <c r="F33" s="25" t="s">
@@ -2441,7 +2439,7 @@
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
     </row>
-    <row r="34" spans="4:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D34" s="24"/>
       <c r="E34" s="24"/>
       <c r="F34" s="25" t="s">
@@ -2460,7 +2458,7 @@
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
     </row>
-    <row r="35" spans="4:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D35" s="24"/>
       <c r="E35" s="24"/>
       <c r="F35" s="25" t="s">
@@ -2478,23 +2476,23 @@
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
-      <c r="W35" s="37" t="s">
+      <c r="W35" s="36" t="s">
         <v>269</v>
       </c>
-      <c r="X35" s="38" t="s">
+      <c r="X35" s="37" t="s">
         <v>270</v>
       </c>
-      <c r="Y35" s="38" t="s">
+      <c r="Y35" s="37" t="s">
         <v>271</v>
       </c>
-      <c r="Z35" s="39" t="s">
+      <c r="Z35" s="38" t="s">
         <v>272</v>
       </c>
-      <c r="AA35" s="39" t="s">
+      <c r="AA35" s="38" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="36" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D36" s="24"/>
       <c r="E36" s="24"/>
       <c r="F36" s="25" t="s">
@@ -2512,23 +2510,23 @@
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
-      <c r="W36" s="40" t="s">
+      <c r="W36" s="39" t="s">
         <v>274</v>
       </c>
-      <c r="X36" s="41">
+      <c r="X36" s="40">
         <v>1.01</v>
       </c>
-      <c r="Y36" s="41">
+      <c r="Y36" s="40">
         <v>55.54</v>
       </c>
-      <c r="Z36" s="42">
+      <c r="Z36" s="41">
         <v>2.7126000271260002</v>
       </c>
-      <c r="AA36" s="43" t="s">
+      <c r="AA36" s="42" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="37" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D37" s="24"/>
       <c r="E37" s="24"/>
       <c r="F37" s="25" t="s">
@@ -2547,7 +2545,7 @@
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
     </row>
-    <row r="38" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D38" s="24"/>
       <c r="E38" s="24"/>
       <c r="F38" s="25" t="s">
@@ -2566,7 +2564,7 @@
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
     </row>
-    <row r="39" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D39" s="24"/>
       <c r="E39" s="24"/>
       <c r="F39" s="25" t="s">
@@ -2585,7 +2583,7 @@
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
     </row>
-    <row r="40" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D40" s="24"/>
       <c r="E40" s="24"/>
       <c r="F40" s="25" t="s">
@@ -2604,7 +2602,7 @@
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
     </row>
-    <row r="41" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D41" s="24"/>
       <c r="E41" s="24"/>
       <c r="F41" s="25" t="s">
@@ -2623,7 +2621,7 @@
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
     </row>
-    <row r="42" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D42" s="24"/>
       <c r="E42" s="24"/>
       <c r="F42" s="25" t="s">
@@ -2648,7 +2646,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="43" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D43" s="24"/>
       <c r="E43" s="24"/>
       <c r="F43" s="25" t="s">
@@ -2671,7 +2669,7 @@
         <v>18.432500000000001</v>
       </c>
     </row>
-    <row r="44" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D44" s="24"/>
       <c r="E44" s="24"/>
       <c r="F44" s="25" t="s">
@@ -2690,7 +2688,7 @@
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
     </row>
-    <row r="45" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D45" s="24"/>
       <c r="E45" s="24"/>
       <c r="F45" s="25" t="s">
@@ -2709,7 +2707,7 @@
       <c r="K45" s="4"/>
       <c r="L45" s="4"/>
     </row>
-    <row r="46" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D46" s="24"/>
       <c r="E46" s="24"/>
       <c r="F46" s="25" t="s">
@@ -2728,7 +2726,7 @@
       <c r="K46" s="4"/>
       <c r="L46" s="4"/>
     </row>
-    <row r="47" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D47" s="24"/>
       <c r="E47" s="24"/>
       <c r="F47" s="25" t="s">
@@ -2753,7 +2751,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="4:27" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D48" s="24"/>
       <c r="E48" s="24"/>
       <c r="F48" s="25" t="s">
@@ -2792,11 +2790,11 @@
       <c r="Y48" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="Z48" s="36" t="s">
+      <c r="Z48" s="35" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="49" spans="4:26" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D49" s="24" t="s">
         <v>260</v>
       </c>
@@ -2843,7 +2841,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="50" spans="4:26" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
       <c r="F50" s="5"/>
@@ -2854,7 +2852,7 @@
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
     </row>
-    <row r="51" spans="4:26" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
       <c r="F51" s="5"/>
@@ -2865,7 +2863,7 @@
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
     </row>
-    <row r="52" spans="4:26" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
       <c r="F52" s="5"/>
@@ -2876,7 +2874,7 @@
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
     </row>
-    <row r="53" spans="4:26" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
       <c r="F53" s="5"/>
@@ -2887,12 +2885,12 @@
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
     </row>
-    <row r="55" spans="4:26" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D55" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="4:26" x14ac:dyDescent="0.3">
+    <row r="56" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D56" s="1" t="s">
         <v>0</v>
       </c>
@@ -2921,7 +2919,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="4:26" ht="42.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="4:26" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="3" t="s">
         <v>9</v>
       </c>
@@ -2950,7 +2948,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="4:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="4:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="3" t="s">
         <v>18</v>
       </c>
@@ -2963,7 +2961,7 @@
       <c r="K58" s="3"/>
       <c r="L58" s="3"/>
     </row>
-    <row r="59" spans="4:26" x14ac:dyDescent="0.3">
+    <row r="59" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D59" s="25" t="s">
         <v>88</v>
       </c>
@@ -2981,7 +2979,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="60" spans="4:26" x14ac:dyDescent="0.3">
+    <row r="60" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D60" s="25"/>
       <c r="E60" s="25"/>
       <c r="F60" s="25" t="s">
@@ -2997,7 +2995,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="61" spans="4:26" x14ac:dyDescent="0.3">
+    <row r="61" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D61" s="25"/>
       <c r="E61" s="25"/>
       <c r="F61" s="25" t="s">
@@ -3013,7 +3011,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="62" spans="4:26" x14ac:dyDescent="0.3">
+    <row r="62" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D62" s="25"/>
       <c r="E62" s="25"/>
       <c r="F62" s="25" t="s">
@@ -3029,7 +3027,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="4:26" x14ac:dyDescent="0.3">
+    <row r="63" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D63" s="25"/>
       <c r="E63" s="25"/>
       <c r="F63" s="25" t="s">
@@ -3045,7 +3043,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="4:26" x14ac:dyDescent="0.3">
+    <row r="64" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D64" s="25"/>
       <c r="E64" s="25"/>
       <c r="F64" s="25" t="s">
@@ -3061,7 +3059,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D65" s="25"/>
       <c r="E65" s="25"/>
       <c r="F65" s="25" t="s">
@@ -3077,7 +3075,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="66" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D66" s="25"/>
       <c r="E66" s="25"/>
       <c r="F66" s="25" t="s">
@@ -3093,7 +3091,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="67" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D67" s="25"/>
       <c r="E67" s="25"/>
       <c r="F67" s="25" t="s">
@@ -3109,7 +3107,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="68" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D68" s="25"/>
       <c r="E68" s="25"/>
       <c r="F68" s="25" t="s">
@@ -3125,7 +3123,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="69" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D69" s="25"/>
       <c r="E69" s="25"/>
       <c r="F69" s="25" t="s">
@@ -3141,7 +3139,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="70" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D70" s="25"/>
       <c r="E70" s="25"/>
       <c r="F70" s="25" t="s">
@@ -3157,7 +3155,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="71" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D71" s="25"/>
       <c r="E71" s="25"/>
       <c r="F71" s="25" t="s">
@@ -3173,7 +3171,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="72" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D72" s="25"/>
       <c r="E72" s="25"/>
       <c r="F72" s="25" t="s">
@@ -3189,7 +3187,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="73" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D73" s="25"/>
       <c r="E73" s="25"/>
       <c r="F73" s="25" t="s">
@@ -3205,7 +3203,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D74" s="25"/>
       <c r="E74" s="25"/>
       <c r="F74" s="25" t="s">
@@ -3221,7 +3219,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D75" s="25"/>
       <c r="E75" s="25"/>
       <c r="F75" s="25" t="s">
@@ -3237,7 +3235,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="76" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D76" s="25"/>
       <c r="E76" s="25"/>
       <c r="F76" s="25" t="s">
@@ -3253,7 +3251,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="77" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D77" s="25"/>
       <c r="E77" s="25"/>
       <c r="F77" s="25" t="s">
@@ -3269,7 +3267,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="78" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D78" s="25"/>
       <c r="E78" s="25"/>
       <c r="F78" s="25" t="s">
@@ -3285,7 +3283,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="79" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D79" s="25"/>
       <c r="E79" s="25"/>
       <c r="F79" s="25" t="s">
@@ -3301,7 +3299,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="80" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D80" s="25"/>
       <c r="E80" s="25"/>
       <c r="F80" s="25" t="s">
@@ -3317,7 +3315,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="81" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D81" s="25"/>
       <c r="E81" s="25"/>
       <c r="F81" s="25" t="s">
@@ -3333,7 +3331,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="82" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D82" s="25"/>
       <c r="E82" s="25"/>
       <c r="F82" s="25" t="s">
@@ -3349,7 +3347,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="83" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D83" s="25"/>
       <c r="E83" s="25"/>
       <c r="F83" s="25" t="s">
@@ -3365,7 +3363,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="84" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D84" s="25"/>
       <c r="E84" s="25"/>
       <c r="F84" s="25" t="s">
@@ -3381,7 +3379,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="85" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D85" s="25"/>
       <c r="E85" s="25"/>
       <c r="F85" s="25" t="s">
@@ -3397,7 +3395,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="86" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D86" s="25"/>
       <c r="E86" s="25"/>
       <c r="F86" s="25" t="s">
@@ -3413,7 +3411,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="87" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="4:9" x14ac:dyDescent="0.25">
       <c r="F87" s="25" t="s">
         <v>230</v>
       </c>
@@ -3427,7 +3425,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="88" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="4:9" x14ac:dyDescent="0.25">
       <c r="F88" s="25" t="s">
         <v>232</v>
       </c>
@@ -3441,7 +3439,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="89" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="4:9" x14ac:dyDescent="0.25">
       <c r="F89" s="25" t="s">
         <v>234</v>
       </c>
@@ -3455,7 +3453,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="90" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="4:9" x14ac:dyDescent="0.25">
       <c r="F90" s="25" t="s">
         <v>236</v>
       </c>
@@ -3469,7 +3467,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="4:9" x14ac:dyDescent="0.25">
       <c r="F91" s="25" t="s">
         <v>238</v>
       </c>
@@ -3483,7 +3481,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="4:9" x14ac:dyDescent="0.25">
       <c r="F92" s="25" t="s">
         <v>240</v>
       </c>
@@ -3497,7 +3495,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="93" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="4:9" x14ac:dyDescent="0.25">
       <c r="F93" s="25" t="s">
         <v>242</v>
       </c>
@@ -3511,7 +3509,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="94" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="4:9" x14ac:dyDescent="0.25">
       <c r="F94" s="25" t="s">
         <v>244</v>
       </c>
@@ -3525,7 +3523,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="95" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="4:9" x14ac:dyDescent="0.25">
       <c r="F95" s="25" t="s">
         <v>246</v>
       </c>
@@ -3539,7 +3537,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="96" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="4:9" x14ac:dyDescent="0.25">
       <c r="F96" s="25" t="s">
         <v>248</v>
       </c>
@@ -3553,7 +3551,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="97" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F97" s="25" t="s">
         <v>250</v>
       </c>
@@ -3567,7 +3565,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="98" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F98" s="25" t="s">
         <v>252</v>
       </c>
@@ -3581,7 +3579,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="99" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F99" s="25" t="s">
         <v>254</v>
       </c>
@@ -3595,7 +3593,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="100" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F100" s="25" t="s">
         <v>256</v>
       </c>
@@ -3609,37 +3607,37 @@
         <v>89</v>
       </c>
     </row>
-    <row r="101" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F101" s="25"/>
       <c r="G101" s="25"/>
       <c r="H101" s="24"/>
       <c r="I101" s="24"/>
     </row>
-    <row r="102" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F102" s="25"/>
       <c r="G102" s="25"/>
       <c r="H102" s="24"/>
       <c r="I102" s="24"/>
     </row>
-    <row r="103" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F103" s="25"/>
       <c r="G103" s="25"/>
       <c r="H103" s="24"/>
       <c r="I103" s="24"/>
     </row>
-    <row r="104" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="104" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F104" s="25"/>
       <c r="G104" s="25"/>
       <c r="H104" s="24"/>
       <c r="I104" s="24"/>
     </row>
-    <row r="105" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="105" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F105" s="25"/>
       <c r="G105" s="25"/>
       <c r="H105" s="24"/>
       <c r="I105" s="24"/>
     </row>
-    <row r="106" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="106" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F106" s="25"/>
       <c r="G106" s="25"/>
       <c r="H106" s="24"/>
@@ -3656,21 +3654,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C8789E0-9FF6-48FA-AD50-A4FA3DA5E255}">
   <dimension ref="B2:P52"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11:L52"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.88671875" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="7" max="7" width="15.5546875" customWidth="1"/>
-    <col min="14" max="14" width="30.44140625" customWidth="1"/>
-    <col min="16" max="16" width="17.5546875" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="14" max="14" width="30.42578125" customWidth="1"/>
+    <col min="16" max="16" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="N2" s="20" t="s">
         <v>67</v>
       </c>
@@ -3678,7 +3676,7 @@
         <v>75.166375708662926</v>
       </c>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="N3" s="20" t="s">
         <v>68</v>
       </c>
@@ -3686,7 +3684,7 @@
         <v>77.841777688967127</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="N4" s="20" t="s">
         <v>69</v>
       </c>
@@ -3694,7 +3692,7 @@
         <v>55.539114956987063</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="N5" s="20" t="s">
         <v>80</v>
       </c>
@@ -3702,7 +3700,7 @@
         <v>78.281203343664757</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>20</v>
       </c>
@@ -3724,7 +3722,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="2:16" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:16" ht="23.25" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>30</v>
       </c>
@@ -3747,7 +3745,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
         <v>37</v>
       </c>
@@ -3755,7 +3753,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="12" t="s">
         <v>2</v>
       </c>
@@ -3799,15 +3797,15 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <f>'COMM&amp;PROCESS'!F7</f>
         <v>AUTO-NE-DSL1-CAM1</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="43" t="s">
         <v>46</v>
       </c>
       <c r="E11" s="26">
@@ -3846,7 +3844,7 @@
         <v>197.80625186490244</v>
       </c>
     </row>
-    <row r="12" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <f>'COMM&amp;PROCESS'!F8</f>
         <v>AUTO-NE-HFO1-CAM1</v>
@@ -3854,7 +3852,7 @@
       <c r="C12" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="33" t="s">
+      <c r="D12" s="43" t="s">
         <v>46</v>
       </c>
       <c r="E12" s="26">
@@ -3893,7 +3891,7 @@
         <v>223.66058098189933</v>
       </c>
     </row>
-    <row r="13" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <f>'COMM&amp;PROCESS'!F9</f>
         <v>AUTO-NE-OIL1-CAM1</v>
@@ -3901,7 +3899,7 @@
       <c r="C13" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="33" t="s">
+      <c r="D13" s="43" t="s">
         <v>46</v>
       </c>
       <c r="E13" s="26">
@@ -3940,7 +3938,7 @@
         <v>222.40507911133466</v>
       </c>
     </row>
-    <row r="14" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" t="str">
         <f>'COMM&amp;PROCESS'!F10</f>
         <v>AUTO-NE-GASCT1-CAM1</v>
@@ -3948,7 +3946,7 @@
       <c r="C14" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="33" t="s">
+      <c r="D14" s="43" t="s">
         <v>46</v>
       </c>
       <c r="E14" s="26">
@@ -3987,7 +3985,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="15" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
         <f>'COMM&amp;PROCESS'!F11</f>
         <v>AUTO-NE-GASCT2-CAM1</v>
@@ -3995,7 +3993,7 @@
       <c r="C15" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="33" t="s">
+      <c r="D15" s="43" t="s">
         <v>46</v>
       </c>
       <c r="E15" s="30">
@@ -4034,7 +4032,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="16" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" t="str">
         <f>'COMM&amp;PROCESS'!F12</f>
         <v>AUTO-NE-GASCT3-CAM1</v>
@@ -4042,7 +4040,7 @@
       <c r="C16" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="33" t="s">
+      <c r="D16" s="43" t="s">
         <v>46</v>
       </c>
       <c r="E16" s="26">
@@ -4081,15 +4079,15 @@
         <v>157.7815765823496</v>
       </c>
     </row>
-    <row r="17" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" t="str">
         <f>'COMM&amp;PROCESS'!F13</f>
         <v>AUTO-NE-DSL1-CAM2</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="43" t="s">
         <v>47</v>
       </c>
       <c r="E17" s="26">
@@ -4128,7 +4126,7 @@
         <v>197.80625186490244</v>
       </c>
     </row>
-    <row r="18" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f>'COMM&amp;PROCESS'!F14</f>
         <v>AUTO-NE-HFO1-CAM2</v>
@@ -4136,7 +4134,7 @@
       <c r="C18" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="33" t="s">
+      <c r="D18" s="43" t="s">
         <v>47</v>
       </c>
       <c r="E18" s="26">
@@ -4175,7 +4173,7 @@
         <v>223.66058098189933</v>
       </c>
     </row>
-    <row r="19" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f>'COMM&amp;PROCESS'!F15</f>
         <v>AUTO-NE-OIL1-CAM2</v>
@@ -4183,7 +4181,7 @@
       <c r="C19" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="43" t="s">
         <v>47</v>
       </c>
       <c r="E19" s="26">
@@ -4222,7 +4220,7 @@
         <v>222.40507911133466</v>
       </c>
     </row>
-    <row r="20" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f>'COMM&amp;PROCESS'!F16</f>
         <v>AUTO-NE-GASCT1-CAM2</v>
@@ -4230,7 +4228,7 @@
       <c r="C20" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="33" t="s">
+      <c r="D20" s="43" t="s">
         <v>47</v>
       </c>
       <c r="E20" s="26">
@@ -4269,7 +4267,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="21" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
         <f>'COMM&amp;PROCESS'!F17</f>
         <v>AUTO-NE-GASCT2-CAM2</v>
@@ -4277,7 +4275,7 @@
       <c r="C21" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="33" t="s">
+      <c r="D21" s="43" t="s">
         <v>47</v>
       </c>
       <c r="E21" s="30">
@@ -4316,7 +4314,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="22" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
         <f>'COMM&amp;PROCESS'!F18</f>
         <v>AUTO-NE-GASCT3-CAM2</v>
@@ -4324,7 +4322,7 @@
       <c r="C22" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="33" t="s">
+      <c r="D22" s="43" t="s">
         <v>47</v>
       </c>
       <c r="E22" s="26">
@@ -4363,7 +4361,7 @@
         <v>157.7815765823496</v>
       </c>
     </row>
-    <row r="23" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
         <f>'COMM&amp;PROCESS'!F19</f>
         <v>AUTO-NE-DSL1-CAM3</v>
@@ -4371,7 +4369,7 @@
       <c r="C23" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D23" s="33" t="s">
+      <c r="D23" s="43" t="s">
         <v>48</v>
       </c>
       <c r="E23" s="26">
@@ -4395,7 +4393,7 @@
       <c r="K23" s="18">
         <v>31.536000000000001</v>
       </c>
-      <c r="L23" s="35">
+      <c r="L23" s="34">
         <v>2022</v>
       </c>
       <c r="N23" t="str">
@@ -4410,7 +4408,7 @@
         <v>197.80625186490244</v>
       </c>
     </row>
-    <row r="24" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
         <f>'COMM&amp;PROCESS'!F20</f>
         <v>AUTO-NE-HFO1-CAM3</v>
@@ -4418,7 +4416,7 @@
       <c r="C24" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D24" s="33" t="s">
+      <c r="D24" s="43" t="s">
         <v>48</v>
       </c>
       <c r="E24" s="26">
@@ -4442,7 +4440,7 @@
       <c r="K24" s="18">
         <v>31.536000000000001</v>
       </c>
-      <c r="L24" s="35">
+      <c r="L24" s="34">
         <v>2022</v>
       </c>
       <c r="N24" t="str">
@@ -4457,7 +4455,7 @@
         <v>223.66058098189933</v>
       </c>
     </row>
-    <row r="25" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" t="str">
         <f>'COMM&amp;PROCESS'!F21</f>
         <v>AUTO-NE-OIL1-CAM3</v>
@@ -4465,10 +4463,10 @@
       <c r="C25" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D25" s="33" t="s">
+      <c r="D25" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="E25" s="34">
+      <c r="E25" s="33">
         <v>0.38</v>
       </c>
       <c r="F25" s="27">
@@ -4489,7 +4487,7 @@
       <c r="K25" s="18">
         <v>31.536000000000001</v>
       </c>
-      <c r="L25" s="35">
+      <c r="L25" s="34">
         <v>2022</v>
       </c>
       <c r="N25" t="str">
@@ -4504,7 +4502,7 @@
         <v>204.84678339201875</v>
       </c>
     </row>
-    <row r="26" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" t="str">
         <f>'COMM&amp;PROCESS'!F22</f>
         <v>AUTO-NE-GASCT1-CAM3</v>
@@ -4512,7 +4510,7 @@
       <c r="C26" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D26" s="33" t="s">
+      <c r="D26" s="43" t="s">
         <v>48</v>
       </c>
       <c r="E26" s="26">
@@ -4536,7 +4534,7 @@
       <c r="K26" s="18">
         <v>31.536000000000001</v>
       </c>
-      <c r="L26" s="35">
+      <c r="L26" s="34">
         <v>2022</v>
       </c>
       <c r="N26" t="str">
@@ -4551,7 +4549,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="27" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" t="str">
         <f>'COMM&amp;PROCESS'!F23</f>
         <v>AUTO-NE-GASCT2-CAM3</v>
@@ -4559,7 +4557,7 @@
       <c r="C27" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D27" s="33" t="s">
+      <c r="D27" s="43" t="s">
         <v>48</v>
       </c>
       <c r="E27" s="30">
@@ -4598,7 +4596,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="28" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" t="str">
         <f>'COMM&amp;PROCESS'!F24</f>
         <v>AUTO-NE-GASCT3-CAM3</v>
@@ -4606,7 +4604,7 @@
       <c r="C28" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="33" t="s">
+      <c r="D28" s="43" t="s">
         <v>48</v>
       </c>
       <c r="E28" s="26">
@@ -4645,7 +4643,7 @@
         <v>157.7815765823496</v>
       </c>
     </row>
-    <row r="29" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" t="str">
         <f>'COMM&amp;PROCESS'!F25</f>
         <v>AUTO-NE-DSL1-CAM4</v>
@@ -4653,7 +4651,7 @@
       <c r="C29" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D29" s="33" t="s">
+      <c r="D29" s="43" t="s">
         <v>49</v>
       </c>
       <c r="E29" s="26">
@@ -4692,7 +4690,7 @@
         <v>197.80625186490244</v>
       </c>
     </row>
-    <row r="30" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" t="str">
         <f>'COMM&amp;PROCESS'!F26</f>
         <v>AUTO-NE-HFO1-CAM4</v>
@@ -4700,7 +4698,7 @@
       <c r="C30" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D30" s="33" t="s">
+      <c r="D30" s="43" t="s">
         <v>49</v>
       </c>
       <c r="E30" s="26">
@@ -4739,7 +4737,7 @@
         <v>223.66058098189933</v>
       </c>
     </row>
-    <row r="31" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" t="str">
         <f>'COMM&amp;PROCESS'!F27</f>
         <v>AUTO-NE-OIL1-CAM4</v>
@@ -4747,7 +4745,7 @@
       <c r="C31" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D31" s="33" t="s">
+      <c r="D31" s="43" t="s">
         <v>49</v>
       </c>
       <c r="E31" s="26">
@@ -4786,7 +4784,7 @@
         <v>222.40507911133466</v>
       </c>
     </row>
-    <row r="32" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" t="str">
         <f>'COMM&amp;PROCESS'!F28</f>
         <v>AUTO-NE-GASCT1-CAM4</v>
@@ -4794,7 +4792,7 @@
       <c r="C32" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D32" s="33" t="s">
+      <c r="D32" s="43" t="s">
         <v>49</v>
       </c>
       <c r="E32" s="26">
@@ -4833,7 +4831,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="33" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" t="str">
         <f>'COMM&amp;PROCESS'!F29</f>
         <v>AUTO-NE-GASCT2-CAM4</v>
@@ -4841,7 +4839,7 @@
       <c r="C33" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D33" s="33" t="s">
+      <c r="D33" s="43" t="s">
         <v>49</v>
       </c>
       <c r="E33" s="30">
@@ -4880,7 +4878,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="34" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" t="str">
         <f>'COMM&amp;PROCESS'!F30</f>
         <v>AUTO-NE-GASCT3-CAM4</v>
@@ -4888,7 +4886,7 @@
       <c r="C34" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="33" t="s">
+      <c r="D34" s="43" t="s">
         <v>49</v>
       </c>
       <c r="E34" s="26">
@@ -4927,7 +4925,7 @@
         <v>157.7815765823496</v>
       </c>
     </row>
-    <row r="35" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B35" t="str">
         <f>'COMM&amp;PROCESS'!F31</f>
         <v>AUTO-NE-DSL1-CAM5</v>
@@ -4935,7 +4933,7 @@
       <c r="C35" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D35" s="33" t="s">
+      <c r="D35" s="43" t="s">
         <v>50</v>
       </c>
       <c r="E35" s="26">
@@ -4974,7 +4972,7 @@
         <v>197.80625186490244</v>
       </c>
     </row>
-    <row r="36" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" t="str">
         <f>'COMM&amp;PROCESS'!F32</f>
         <v>AUTO-NE-HFO1-CAM5</v>
@@ -4982,7 +4980,7 @@
       <c r="C36" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D36" s="33" t="s">
+      <c r="D36" s="43" t="s">
         <v>50</v>
       </c>
       <c r="E36" s="26">
@@ -5021,7 +5019,7 @@
         <v>223.66058098189933</v>
       </c>
     </row>
-    <row r="37" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
         <f>'COMM&amp;PROCESS'!F33</f>
         <v>AUTO-NE-OIL1-CAM5</v>
@@ -5029,7 +5027,7 @@
       <c r="C37" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D37" s="33" t="s">
+      <c r="D37" s="43" t="s">
         <v>50</v>
       </c>
       <c r="E37" s="26">
@@ -5068,7 +5066,7 @@
         <v>222.40507911133466</v>
       </c>
     </row>
-    <row r="38" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" t="str">
         <f>'COMM&amp;PROCESS'!F34</f>
         <v>AUTO-NE-GASCT1-CAM5</v>
@@ -5076,7 +5074,7 @@
       <c r="C38" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D38" s="33" t="s">
+      <c r="D38" s="43" t="s">
         <v>50</v>
       </c>
       <c r="E38" s="26">
@@ -5115,7 +5113,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="39" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
         <f>'COMM&amp;PROCESS'!F35</f>
         <v>AUTO-NE-GASCT2-CAM5</v>
@@ -5123,7 +5121,7 @@
       <c r="C39" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D39" s="33" t="s">
+      <c r="D39" s="43" t="s">
         <v>50</v>
       </c>
       <c r="E39" s="30">
@@ -5162,7 +5160,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="40" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
         <f>'COMM&amp;PROCESS'!F36</f>
         <v>AUTO-NE-GASCT3-CAM5</v>
@@ -5170,7 +5168,7 @@
       <c r="C40" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D40" s="33" t="s">
+      <c r="D40" s="43" t="s">
         <v>50</v>
       </c>
       <c r="E40" s="26">
@@ -5209,7 +5207,7 @@
         <v>157.7815765823496</v>
       </c>
     </row>
-    <row r="41" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" t="str">
         <f>'COMM&amp;PROCESS'!F37</f>
         <v>AUTO-NE-DSL1-CAM6</v>
@@ -5217,7 +5215,7 @@
       <c r="C41" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D41" s="33" t="s">
+      <c r="D41" s="43" t="s">
         <v>51</v>
       </c>
       <c r="E41" s="26">
@@ -5256,7 +5254,7 @@
         <v>197.80625186490244</v>
       </c>
     </row>
-    <row r="42" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B42" t="str">
         <f>'COMM&amp;PROCESS'!F38</f>
         <v>AUTO-NE-HFO1-CAM6</v>
@@ -5264,7 +5262,7 @@
       <c r="C42" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D42" s="33" t="s">
+      <c r="D42" s="43" t="s">
         <v>51</v>
       </c>
       <c r="E42" s="26">
@@ -5303,7 +5301,7 @@
         <v>223.66058098189933</v>
       </c>
     </row>
-    <row r="43" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B43" t="str">
         <f>'COMM&amp;PROCESS'!F39</f>
         <v>AUTO-NE-OIL1-CAM6</v>
@@ -5311,7 +5309,7 @@
       <c r="C43" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D43" s="33" t="s">
+      <c r="D43" s="43" t="s">
         <v>51</v>
       </c>
       <c r="E43" s="26">
@@ -5350,7 +5348,7 @@
         <v>222.40507911133466</v>
       </c>
     </row>
-    <row r="44" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B44" t="str">
         <f>'COMM&amp;PROCESS'!F40</f>
         <v>AUTO-NE-GASCT1-CAM6</v>
@@ -5358,7 +5356,7 @@
       <c r="C44" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D44" s="33" t="s">
+      <c r="D44" s="43" t="s">
         <v>51</v>
       </c>
       <c r="E44" s="26">
@@ -5397,7 +5395,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="45" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" t="str">
         <f>'COMM&amp;PROCESS'!F41</f>
         <v>AUTO-NE-GASCT2-CAM6</v>
@@ -5405,7 +5403,7 @@
       <c r="C45" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D45" s="33" t="s">
+      <c r="D45" s="43" t="s">
         <v>51</v>
       </c>
       <c r="E45" s="30">
@@ -5444,7 +5442,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="46" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" t="str">
         <f>'COMM&amp;PROCESS'!F42</f>
         <v>AUTO-NE-GASCT3-CAM6</v>
@@ -5452,7 +5450,7 @@
       <c r="C46" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D46" s="33" t="s">
+      <c r="D46" s="43" t="s">
         <v>51</v>
       </c>
       <c r="E46" s="26">
@@ -5491,7 +5489,7 @@
         <v>157.7815765823496</v>
       </c>
     </row>
-    <row r="47" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B47" t="str">
         <f>'COMM&amp;PROCESS'!F43</f>
         <v>AUTO-NE-DSL1-CAM7</v>
@@ -5499,7 +5497,7 @@
       <c r="C47" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D47" s="33" t="s">
+      <c r="D47" s="43" t="s">
         <v>52</v>
       </c>
       <c r="E47" s="26">
@@ -5538,7 +5536,7 @@
         <v>197.80625186490244</v>
       </c>
     </row>
-    <row r="48" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B48" t="str">
         <f>'COMM&amp;PROCESS'!F44</f>
         <v>AUTO-NE-HFO1-CAM7</v>
@@ -5546,7 +5544,7 @@
       <c r="C48" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D48" s="33" t="s">
+      <c r="D48" s="43" t="s">
         <v>52</v>
       </c>
       <c r="E48" s="26">
@@ -5585,7 +5583,7 @@
         <v>223.66058098189933</v>
       </c>
     </row>
-    <row r="49" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B49" t="str">
         <f>'COMM&amp;PROCESS'!F45</f>
         <v>AUTO-NE-OIL1-CAM7</v>
@@ -5593,7 +5591,7 @@
       <c r="C49" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D49" s="33" t="s">
+      <c r="D49" s="43" t="s">
         <v>52</v>
       </c>
       <c r="E49" s="26">
@@ -5632,7 +5630,7 @@
         <v>222.40507911133466</v>
       </c>
     </row>
-    <row r="50" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B50" t="str">
         <f>'COMM&amp;PROCESS'!F46</f>
         <v>AUTO-NE-GASCT1-CAM7</v>
@@ -5640,7 +5638,7 @@
       <c r="C50" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D50" s="33" t="s">
+      <c r="D50" s="43" t="s">
         <v>52</v>
       </c>
       <c r="E50" s="26">
@@ -5679,7 +5677,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="51" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B51" t="str">
         <f>'COMM&amp;PROCESS'!F47</f>
         <v>AUTO-NE-GASCT2-CAM7</v>
@@ -5687,7 +5685,7 @@
       <c r="C51" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D51" s="33" t="s">
+      <c r="D51" s="43" t="s">
         <v>52</v>
       </c>
       <c r="E51" s="30">
@@ -5726,7 +5724,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="52" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B52" t="str">
         <f>'COMM&amp;PROCESS'!F48</f>
         <v>AUTO-NE-GASCT3-CAM7</v>
@@ -5734,7 +5732,7 @@
       <c r="C52" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D52" s="33" t="s">
+      <c r="D52" s="43" t="s">
         <v>52</v>
       </c>
       <c r="E52" s="26">
@@ -5783,21 +5781,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB379A20-D2EF-42C3-B504-D06C0353F382}">
   <dimension ref="B2:P52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11:L52"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.88671875" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="7" max="7" width="15.5546875" customWidth="1"/>
-    <col min="14" max="14" width="30.44140625" customWidth="1"/>
-    <col min="16" max="16" width="17.5546875" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="14" max="14" width="30.42578125" customWidth="1"/>
+    <col min="16" max="16" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="N2" s="20" t="s">
         <v>67</v>
       </c>
@@ -5805,7 +5803,7 @@
         <v>75.166375708662926</v>
       </c>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="N3" s="20" t="s">
         <v>68</v>
       </c>
@@ -5813,7 +5811,7 @@
         <v>77.841777688967127</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="N4" s="20" t="s">
         <v>69</v>
       </c>
@@ -5821,7 +5819,7 @@
         <v>55.539114956987063</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="N5" s="20" t="s">
         <v>80</v>
       </c>
@@ -5829,7 +5827,7 @@
         <v>78.281203343664757</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>20</v>
       </c>
@@ -5851,7 +5849,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="2:16" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:16" ht="23.25" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>30</v>
       </c>
@@ -5874,7 +5872,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
         <v>37</v>
       </c>
@@ -5882,7 +5880,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="12" t="s">
         <v>2</v>
       </c>
@@ -5926,7 +5924,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <f>'COMM&amp;PROCESS'!F59</f>
         <v>AUTOCOL-NE-DSL1-CAM1</v>
@@ -5973,7 +5971,7 @@
         <v>197.80625186490244</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <f>'COMM&amp;PROCESS'!F60</f>
         <v>AUTOCOL-NE-HFO1-CAM1</v>
@@ -6020,7 +6018,7 @@
         <v>223.66058098189933</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <f>'COMM&amp;PROCESS'!F61</f>
         <v>AUTOCOL-NE-OIL1-CAM1</v>
@@ -6067,7 +6065,7 @@
         <v>222.40507911133466</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" t="str">
         <f>'COMM&amp;PROCESS'!F62</f>
         <v>AUTOCOL-NE-GASCT1-CAM1</v>
@@ -6114,7 +6112,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
         <f>'COMM&amp;PROCESS'!F63</f>
         <v>AUTOCOL-NE-GASCT2-CAM1</v>
@@ -6161,7 +6159,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" t="str">
         <f>'COMM&amp;PROCESS'!F64</f>
         <v>AUTOCOL-NE-GASCT3-CAM1</v>
@@ -6208,7 +6206,7 @@
         <v>157.7815765823496</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" t="str">
         <f>'COMM&amp;PROCESS'!F65</f>
         <v>AUTOCOL-NE-DSL1-CAM2</v>
@@ -6255,7 +6253,7 @@
         <v>197.80625186490244</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f>'COMM&amp;PROCESS'!F66</f>
         <v>AUTOCOL-NE-HFO1-CAM2</v>
@@ -6302,7 +6300,7 @@
         <v>223.66058098189933</v>
       </c>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f>'COMM&amp;PROCESS'!F67</f>
         <v>AUTOCOL-NE-OIL1-CAM2</v>
@@ -6349,7 +6347,7 @@
         <v>222.40507911133466</v>
       </c>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f>'COMM&amp;PROCESS'!F68</f>
         <v>AUTOCOL-NE-GASCT1-CAM2</v>
@@ -6396,7 +6394,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
         <f>'COMM&amp;PROCESS'!F69</f>
         <v>AUTOCOL-NE-GASCT2-CAM2</v>
@@ -6443,7 +6441,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
         <f>'COMM&amp;PROCESS'!F70</f>
         <v>AUTOCOL-NE-GASCT3-CAM2</v>
@@ -6490,7 +6488,7 @@
         <v>157.7815765823496</v>
       </c>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
         <f>'COMM&amp;PROCESS'!F71</f>
         <v>AUTOCOL-NE-DSL1-CAM3</v>
@@ -6522,7 +6520,7 @@
       <c r="K23" s="18">
         <v>31.536000000000001</v>
       </c>
-      <c r="L23" s="35">
+      <c r="L23" s="34">
         <v>2022</v>
       </c>
       <c r="N23" t="str">
@@ -6537,7 +6535,7 @@
         <v>197.80625186490244</v>
       </c>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
         <f>'COMM&amp;PROCESS'!F72</f>
         <v>AUTOCOL-NE-HFO1-CAM3</v>
@@ -6569,7 +6567,7 @@
       <c r="K24" s="18">
         <v>31.536000000000001</v>
       </c>
-      <c r="L24" s="35">
+      <c r="L24" s="34">
         <v>2022</v>
       </c>
       <c r="N24" t="str">
@@ -6584,7 +6582,7 @@
         <v>223.66058098189933</v>
       </c>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25" t="str">
         <f>'COMM&amp;PROCESS'!F73</f>
         <v>AUTOCOL-NE-OIL1-CAM3</v>
@@ -6616,7 +6614,7 @@
       <c r="K25" s="18">
         <v>31.536000000000001</v>
       </c>
-      <c r="L25" s="35">
+      <c r="L25" s="34">
         <v>2022</v>
       </c>
       <c r="N25" t="str">
@@ -6631,7 +6629,7 @@
         <v>222.40507911133466</v>
       </c>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B26" t="str">
         <f>'COMM&amp;PROCESS'!F74</f>
         <v>AUTOCOL-NE-GASCT1-CAM3</v>
@@ -6663,7 +6661,7 @@
       <c r="K26" s="18">
         <v>31.536000000000001</v>
       </c>
-      <c r="L26" s="35">
+      <c r="L26" s="34">
         <v>2022</v>
       </c>
       <c r="N26" t="str">
@@ -6678,7 +6676,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" t="str">
         <f>'COMM&amp;PROCESS'!F75</f>
         <v>AUTOCOL-NE-GASCT2-CAM3</v>
@@ -6725,7 +6723,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28" t="str">
         <f>'COMM&amp;PROCESS'!F76</f>
         <v>AUTOCOL-NE-GASCT3-CAM3</v>
@@ -6772,7 +6770,7 @@
         <v>157.7815765823496</v>
       </c>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B29" t="str">
         <f>'COMM&amp;PROCESS'!F77</f>
         <v>AUTOCOL-NE-DSL1-CAM4</v>
@@ -6819,7 +6817,7 @@
         <v>197.80625186490244</v>
       </c>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B30" t="str">
         <f>'COMM&amp;PROCESS'!F78</f>
         <v>AUTOCOL-NE-HFO1-CAM4</v>
@@ -6866,7 +6864,7 @@
         <v>223.66058098189933</v>
       </c>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" t="str">
         <f>'COMM&amp;PROCESS'!F79</f>
         <v>AUTOCOL-NE-OIL1-CAM4</v>
@@ -6913,7 +6911,7 @@
         <v>222.40507911133466</v>
       </c>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B32" t="str">
         <f>'COMM&amp;PROCESS'!F80</f>
         <v>AUTOCOL-NE-GASCT1-CAM4</v>
@@ -6960,7 +6958,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B33" t="str">
         <f>'COMM&amp;PROCESS'!F81</f>
         <v>AUTOCOL-NE-GASCT2-CAM4</v>
@@ -7007,7 +7005,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B34" t="str">
         <f>'COMM&amp;PROCESS'!F82</f>
         <v>AUTOCOL-NE-GASCT3-CAM4</v>
@@ -7054,7 +7052,7 @@
         <v>157.7815765823496</v>
       </c>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B35" t="str">
         <f>'COMM&amp;PROCESS'!F83</f>
         <v>AUTOCOL-NE-DSL1-CAM5</v>
@@ -7101,7 +7099,7 @@
         <v>197.80625186490244</v>
       </c>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B36" t="str">
         <f>'COMM&amp;PROCESS'!F84</f>
         <v>AUTOCOL-NE-HFO1-CAM5</v>
@@ -7148,7 +7146,7 @@
         <v>223.66058098189933</v>
       </c>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
         <f>'COMM&amp;PROCESS'!F85</f>
         <v>AUTOCOL-NE-OIL1-CAM5</v>
@@ -7195,7 +7193,7 @@
         <v>222.40507911133466</v>
       </c>
     </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B38" t="str">
         <f>'COMM&amp;PROCESS'!F86</f>
         <v>AUTOCOL-NE-GASCT1-CAM5</v>
@@ -7242,7 +7240,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
         <f>'COMM&amp;PROCESS'!F87</f>
         <v>AUTOCOL-NE-GASCT2-CAM5</v>
@@ -7289,7 +7287,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
         <f>'COMM&amp;PROCESS'!F88</f>
         <v>AUTOCOL-NE-GASCT3-CAM5</v>
@@ -7336,7 +7334,7 @@
         <v>157.7815765823496</v>
       </c>
     </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B41" t="str">
         <f>'COMM&amp;PROCESS'!F89</f>
         <v>AUTOCOL-NE-DSL1-CAM6</v>
@@ -7383,7 +7381,7 @@
         <v>197.80625186490244</v>
       </c>
     </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B42" t="str">
         <f>'COMM&amp;PROCESS'!F90</f>
         <v>AUTOCOL-NE-HFO1-CAM6</v>
@@ -7430,7 +7428,7 @@
         <v>223.66058098189933</v>
       </c>
     </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43" t="str">
         <f>'COMM&amp;PROCESS'!F91</f>
         <v>AUTOCOL-NE-OIL1-CAM6</v>
@@ -7477,7 +7475,7 @@
         <v>222.40507911133466</v>
       </c>
     </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B44" t="str">
         <f>'COMM&amp;PROCESS'!F92</f>
         <v>AUTOCOL-NE-GASCT1-CAM6</v>
@@ -7524,7 +7522,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B45" t="str">
         <f>'COMM&amp;PROCESS'!F93</f>
         <v>AUTOCOL-NE-GASCT2-CAM6</v>
@@ -7571,7 +7569,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B46" t="str">
         <f>'COMM&amp;PROCESS'!F94</f>
         <v>AUTOCOL-NE-GASCT3-CAM6</v>
@@ -7618,7 +7616,7 @@
         <v>157.7815765823496</v>
       </c>
     </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B47" t="str">
         <f>'COMM&amp;PROCESS'!F95</f>
         <v>AUTOCOL-NE-DSL1-CAM7</v>
@@ -7665,7 +7663,7 @@
         <v>197.80625186490244</v>
       </c>
     </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B48" t="str">
         <f>'COMM&amp;PROCESS'!F96</f>
         <v>AUTOCOL-NE-HFO1-CAM7</v>
@@ -7712,7 +7710,7 @@
         <v>223.66058098189933</v>
       </c>
     </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B49" t="str">
         <f>'COMM&amp;PROCESS'!F97</f>
         <v>AUTOCOL-NE-OIL1-CAM7</v>
@@ -7759,7 +7757,7 @@
         <v>222.40507911133466</v>
       </c>
     </row>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B50" t="str">
         <f>'COMM&amp;PROCESS'!F98</f>
         <v>AUTOCOL-NE-GASCT1-CAM7</v>
@@ -7806,7 +7804,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B51" t="str">
         <f>'COMM&amp;PROCESS'!F99</f>
         <v>AUTOCOL-NE-GASCT2-CAM7</v>
@@ -7853,7 +7851,7 @@
         <v>157.78157658234963</v>
       </c>
     </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B52" t="str">
         <f>'COMM&amp;PROCESS'!F100</f>
         <v>AUTOCOL-NE-GASCT3-CAM7</v>
@@ -7915,9 +7913,9 @@
       <selection activeCell="C6" sqref="C6:Q9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="6" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>22</v>
       </c>
@@ -7964,7 +7962,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="7" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>23</v>
       </c>
@@ -8011,7 +8009,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="8" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>24</v>
       </c>
@@ -8058,7 +8056,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="9" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>25</v>
       </c>

</xml_diff>